<commit_message>
major  refactoring with  JSONPointer
</commit_message>
<xml_diff>
--- a/test/data/assert.xlsx
+++ b/test/data/assert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\.julia\dev\XLSXasJSON\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masterplan\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFEAB19-1FD7-425C-98AA-FED1C07A63E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA72D931-E637-448D-B6FB-7FC62E0780BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dup" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="dup3" sheetId="7" r:id="rId3"/>
     <sheet name="start_line" sheetId="4" r:id="rId4"/>
     <sheet name="empty" sheetId="5" r:id="rId5"/>
+    <sheet name="dict_array" sheetId="8" r:id="rId6"/>
+    <sheet name="array_dict" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,37 +31,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>ColA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>That</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dup(Int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dup(Float)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a.b.c.[1,d]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+  <si>
+    <t>/ColA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ColB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/dup(Int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/dup(Float)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/This</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/That</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/a/b/c/1/d</t>
+  </si>
+  <si>
+    <t>/1/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/a/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cannot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -422,12 +435,12 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,10 +448,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>12</v>
       </c>
@@ -446,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>125</v>
       </c>
@@ -457,7 +470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>555</v>
       </c>
@@ -468,6 +481,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -476,20 +490,20 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>100</v>
       </c>
@@ -509,20 +523,20 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>100</v>
       </c>
@@ -540,21 +554,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C3">
         <v>1</v>
       </c>
@@ -562,7 +576,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C4">
         <v>1</v>
       </c>
@@ -570,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C5">
         <v>3</v>
       </c>
@@ -586,11 +600,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907EC9F1-4DD3-445B-8FB1-B8635EB70877}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3BA1D7-6B37-4D97-B3F1-CB4736F39369}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>